<commit_message>
Tableau stats visites par jour et par langue
</commit_message>
<xml_diff>
--- a/langages.xlsx
+++ b/langages.xlsx
@@ -46,9 +46,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F9"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="0" t="inlineStr">
         <is>
           <t>C</t>
@@ -64,8 +64,23 @@
           <t>1972</t>
         </is>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>c.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="0" t="inlineStr">
         <is>
           <t>Java</t>
@@ -81,8 +96,23 @@
           <t>1995</t>
         </is>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>java.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="0" t="inlineStr">
         <is>
           <t>C++</t>
@@ -98,8 +128,23 @@
           <t>1983</t>
         </is>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>c++.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="0" t="inlineStr">
         <is>
           <t>JavaScript</t>
@@ -115,8 +160,23 @@
           <t>1995</t>
         </is>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>js.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="0" t="inlineStr">
         <is>
           <t>Fox</t>
@@ -132,8 +192,23 @@
           <t>2020</t>
         </is>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>Nouvelle%20description</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>Et%20nouvelle%20utilisation</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>fox.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="0" t="inlineStr">
         <is>
           <t>Ruby</t>
@@ -149,8 +224,26 @@
           <t>1995</t>
         </is>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>Ruby est un langage de programmation libre. Il est interprété, orienté objet et multi-paradigme.
+Ruby est fortement orienté objet et se rapproche ainsi du paradigme objet de Smalltalk.
+Malgré cet aspect exclusivement objet, la programmation procédurale est possible et fréquente. Ruby utilise une syntaxe simple, inspirée par Eiffel et Ada.</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>L'interpréteur officiel, Ruby MRI, fonctionne sur de nombreux systèmes d'exploitation : UNIX, Linux, Microsoft Windows, MS-DOS, OS X, OS/2, ReactOS, AmigaOS, etc. Il est publié sous la double licence libre GNU GPL et la licence Ruby.
+Ruby est fourni avec irb, un interpréteur de commandes interactif pour tester en profondeur le fonctionnement du langage. Il existe une version web d'irb pour tester Ruby dans un navigateur.</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>ruby.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="0" t="inlineStr">
         <is>
           <t>Test%20filtrage</t>
@@ -166,8 +259,23 @@
           <t>2020</t>
         </is>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>Ceci%20est%20une%20description%20pour%20tester%20le%20bon%20fonctionnement%20du%20filtrage%20des%20inputs</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Ceci%20est%20une%20utilisation.%20L%27image%20n%27est%20pas%20en%20rapport%20direct%20avec%20le%20langage%20%28inexistant%2C%20rappelons-le%20%21%29</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>a.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="0" t="inlineStr">
         <is>
           <t>C%23</t>
@@ -181,6 +289,53 @@
       <c r="C8" s="0" t="inlineStr">
         <is>
           <t>2001</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>Non%20disponible</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>Non%20disponible</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>csharp.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>Nouveau truc qui sert pas</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Hy-Vong Georges Dit Rap</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>Ceci est une description pour un test. J&amp;#39;ai en effet remplacé les FILTER_SANITIZE_ENCODED par des FILTER_SANITIZE_STRING pour éviter d&amp;#39;avoir des pourcentages dans mes chaines de caractères</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>Ça, ça sert à rien</t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>rss.png</t>
         </is>
       </c>
     </row>

</xml_diff>